<commit_message>
Update 22.02.18 20:08: Planung Regio
</commit_message>
<xml_diff>
--- a/Mitnehmen.xlsx
+++ b/Mitnehmen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12345" xr2:uid="{90091304-B13A-4F66-81DC-357AE766D936}"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="12345" xr2:uid="{90091304-B13A-4F66-81DC-357AE766D936}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t>Roboter</t>
   </si>
@@ -62,9 +62,6 @@
     <t>BESITZER</t>
   </si>
   <si>
-    <t>Ersatzteile*</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -116,21 +113,6 @@
     <t>Zollstock</t>
   </si>
   <si>
-    <t>Ersatzräder</t>
-  </si>
-  <si>
-    <t>*Details:</t>
-  </si>
-  <si>
-    <t>Nupsis</t>
-  </si>
-  <si>
-    <t>Zahnräder</t>
-  </si>
-  <si>
-    <t>Ersatzbausteine</t>
-  </si>
-  <si>
     <t>College-Block</t>
   </si>
   <si>
@@ -140,12 +122,6 @@
     <t>Schere</t>
   </si>
   <si>
-    <t>EV3</t>
-  </si>
-  <si>
-    <t>HDMI-Kabel</t>
-  </si>
-  <si>
     <t>Vincent</t>
   </si>
   <si>
@@ -155,29 +131,35 @@
     <t>Beide</t>
   </si>
   <si>
-    <t>Eingepackt</t>
-  </si>
-  <si>
-    <t>Besorgt</t>
-  </si>
-  <si>
-    <t>LEGENDE</t>
-  </si>
-  <si>
-    <t>GESAMMELT</t>
-  </si>
-  <si>
-    <t>VORHANDEN</t>
-  </si>
-  <si>
-    <t>ZU HOLEN</t>
+    <t>Im Auto</t>
+  </si>
+  <si>
+    <t>Eingepackt + Wo?</t>
+  </si>
+  <si>
+    <t>Laptoptasche V.</t>
+  </si>
+  <si>
+    <t>Jufo-Tasche 2 F. (Sonstiges)</t>
+  </si>
+  <si>
+    <t>Jufo-Tasche 1 F. (Laptop)</t>
+  </si>
+  <si>
+    <t>Hose V.</t>
+  </si>
+  <si>
+    <t>Jufo-Tasche 1 V. (Verpflegung)</t>
+  </si>
+  <si>
+    <t>Ersatzteile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,13 +177,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,7 +203,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,11 +220,6 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,15 +230,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,16 +249,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -600,22 +572,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8D5E58-4AC6-4F22-92E1-729A9CDC220E}">
-  <dimension ref="B1:I38"/>
+  <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="14.140625" customWidth="1"/>
     <col min="9" max="9" width="46.85546875" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -626,16 +600,17 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -643,18 +618,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6"/>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -662,15 +633,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -678,15 +648,14 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6"/>
-      <c r="I5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -694,15 +663,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -710,15 +678,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -726,15 +693,14 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="I8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -742,12 +708,14 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -755,12 +723,14 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -768,284 +738,314 @@
         <v>2</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>15</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>16</v>
       </c>
       <c r="C15" s="1">
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="6"/>
-      <c r="H15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="H16" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1">
         <v>10</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="H17" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>21</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>22</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>24</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1">
         <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>29</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="7"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>35</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>